<commit_message>
Adding test data for non-deriv transactions
</commit_message>
<xml_diff>
--- a/Testing/TestData/DerivativeTransaction.xlsx
+++ b/Testing/TestData/DerivativeTransaction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\InsidersTradeMonitor\Testing\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{48E649AA-5146-41D0-BB3C-3103AB106544}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7D5A875A-86BB-4100-B231-AD13EE668BD4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
   </bookViews>
@@ -936,7 +936,7 @@
   <dimension ref="A1:Q101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+      <selection activeCell="C63" sqref="A1:Q101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1007,7 +1007,7 @@
       </c>
       <c r="B2">
         <f ca="1">RANDBETWEEN(100001,100030)</f>
-        <v>100011</v>
+        <v>100016</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -1055,7 +1055,7 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B66" ca="1" si="0">RANDBETWEEN(100001,100030)</f>
-        <v>100015</v>
+        <v>100021</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
@@ -1103,7 +1103,7 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>100003</v>
+        <v>100014</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
@@ -1154,7 +1154,7 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>100026</v>
+        <v>100030</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
@@ -1205,7 +1205,7 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>100015</v>
+        <v>100028</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>100002</v>
+        <v>100018</v>
       </c>
       <c r="C7" t="s">
         <v>20</v>
@@ -1307,7 +1307,7 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>100007</v>
+        <v>100001</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
@@ -1358,7 +1358,7 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>100027</v>
+        <v>100020</v>
       </c>
       <c r="C9" t="s">
         <v>17</v>
@@ -1406,7 +1406,7 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>100005</v>
+        <v>100013</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>100005</v>
+        <v>100001</v>
       </c>
       <c r="C11" t="s">
         <v>17</v>
@@ -1505,7 +1505,7 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>100012</v>
+        <v>100009</v>
       </c>
       <c r="C12" t="s">
         <v>22</v>
@@ -1553,7 +1553,7 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>100005</v>
+        <v>100025</v>
       </c>
       <c r="C13" t="s">
         <v>22</v>
@@ -1604,7 +1604,7 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>100004</v>
+        <v>100007</v>
       </c>
       <c r="C14" t="s">
         <v>20</v>
@@ -1655,7 +1655,7 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>100017</v>
+        <v>100003</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
@@ -1706,7 +1706,7 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>100017</v>
+        <v>100007</v>
       </c>
       <c r="C16" t="s">
         <v>17</v>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="I16">
         <f ca="1">RANDBETWEEN(20,300)</f>
-        <v>131</v>
+        <v>197</v>
       </c>
       <c r="J16">
         <v>1</v>
@@ -1744,7 +1744,7 @@
       </c>
       <c r="O16">
         <f ca="1">RANDBETWEEN(200,6000)</f>
-        <v>4700</v>
+        <v>5003</v>
       </c>
       <c r="P16">
         <v>1</v>
@@ -1756,7 +1756,7 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>100029</v>
+        <v>100017</v>
       </c>
       <c r="C17" t="s">
         <v>17</v>
@@ -1778,7 +1778,7 @@
       </c>
       <c r="I17">
         <f t="shared" ref="I17:I29" ca="1" si="1">RANDBETWEEN(20,300)</f>
-        <v>192</v>
+        <v>132</v>
       </c>
       <c r="J17">
         <v>1</v>
@@ -1794,7 +1794,7 @@
       </c>
       <c r="O17">
         <f t="shared" ref="O17:O29" ca="1" si="2">RANDBETWEEN(200,6000)</f>
-        <v>3843</v>
+        <v>2654</v>
       </c>
       <c r="P17">
         <v>1</v>
@@ -1806,7 +1806,7 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>100026</v>
+        <v>100014</v>
       </c>
       <c r="C18" t="s">
         <v>17</v>
@@ -1828,7 +1828,7 @@
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="1"/>
-        <v>281</v>
+        <v>298</v>
       </c>
       <c r="J18">
         <v>1</v>
@@ -1844,7 +1844,7 @@
       </c>
       <c r="O18">
         <f t="shared" ca="1" si="2"/>
-        <v>4350</v>
+        <v>1443</v>
       </c>
       <c r="P18">
         <v>2</v>
@@ -1859,7 +1859,7 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>100002</v>
+        <v>100010</v>
       </c>
       <c r="C19" t="s">
         <v>20</v>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="1"/>
-        <v>82</v>
+        <v>285</v>
       </c>
       <c r="J19">
         <v>1</v>
@@ -1900,7 +1900,7 @@
       </c>
       <c r="O19">
         <f t="shared" ca="1" si="2"/>
-        <v>1585</v>
+        <v>3084</v>
       </c>
       <c r="P19">
         <v>1</v>
@@ -1912,7 +1912,7 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>100003</v>
+        <v>100001</v>
       </c>
       <c r="C20" t="s">
         <v>20</v>
@@ -1934,7 +1934,7 @@
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="1"/>
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="J20">
         <v>1</v>
@@ -1953,7 +1953,7 @@
       </c>
       <c r="O20">
         <f t="shared" ca="1" si="2"/>
-        <v>5364</v>
+        <v>422</v>
       </c>
       <c r="P20">
         <v>1</v>
@@ -1965,7 +1965,7 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>100013</v>
+        <v>100019</v>
       </c>
       <c r="C21" t="s">
         <v>20</v>
@@ -1987,7 +1987,7 @@
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="1"/>
-        <v>168</v>
+        <v>226</v>
       </c>
       <c r="J21">
         <v>1</v>
@@ -2006,7 +2006,7 @@
       </c>
       <c r="O21">
         <f t="shared" ca="1" si="2"/>
-        <v>1495</v>
+        <v>3668</v>
       </c>
       <c r="P21">
         <v>1</v>
@@ -2018,7 +2018,7 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>100004</v>
+        <v>100002</v>
       </c>
       <c r="C22" t="s">
         <v>20</v>
@@ -2040,7 +2040,7 @@
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="1"/>
-        <v>104</v>
+        <v>275</v>
       </c>
       <c r="J22">
         <v>1</v>
@@ -2059,7 +2059,7 @@
       </c>
       <c r="O22">
         <f t="shared" ca="1" si="2"/>
-        <v>717</v>
+        <v>465</v>
       </c>
       <c r="P22">
         <v>1</v>
@@ -2071,7 +2071,7 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>100005</v>
+        <v>100022</v>
       </c>
       <c r="C23" t="s">
         <v>17</v>
@@ -2093,7 +2093,7 @@
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="1"/>
-        <v>38</v>
+        <v>259</v>
       </c>
       <c r="J23">
         <v>1</v>
@@ -2109,7 +2109,7 @@
       </c>
       <c r="O23">
         <f t="shared" ca="1" si="2"/>
-        <v>618</v>
+        <v>3355</v>
       </c>
       <c r="P23">
         <v>1</v>
@@ -2121,7 +2121,7 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>100014</v>
+        <v>100015</v>
       </c>
       <c r="C24" t="s">
         <v>17</v>
@@ -2143,7 +2143,7 @@
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="1"/>
-        <v>175</v>
+        <v>210</v>
       </c>
       <c r="J24">
         <v>1</v>
@@ -2159,7 +2159,7 @@
       </c>
       <c r="O24">
         <f t="shared" ca="1" si="2"/>
-        <v>4954</v>
+        <v>3527</v>
       </c>
       <c r="P24">
         <v>2</v>
@@ -2174,7 +2174,7 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>100015</v>
+        <v>100002</v>
       </c>
       <c r="C25" t="s">
         <v>17</v>
@@ -2196,7 +2196,7 @@
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="1"/>
-        <v>191</v>
+        <v>76</v>
       </c>
       <c r="J25">
         <v>1</v>
@@ -2212,7 +2212,7 @@
       </c>
       <c r="O25">
         <f t="shared" ca="1" si="2"/>
-        <v>4085</v>
+        <v>722</v>
       </c>
       <c r="P25">
         <v>1</v>
@@ -2224,7 +2224,7 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>100006</v>
+        <v>100012</v>
       </c>
       <c r="C26" t="s">
         <v>22</v>
@@ -2246,7 +2246,7 @@
       </c>
       <c r="I26">
         <f t="shared" ca="1" si="1"/>
-        <v>76</v>
+        <v>160</v>
       </c>
       <c r="J26">
         <v>1</v>
@@ -2262,7 +2262,7 @@
       </c>
       <c r="O26">
         <f t="shared" ca="1" si="2"/>
-        <v>653</v>
+        <v>1914</v>
       </c>
       <c r="P26">
         <v>1</v>
@@ -2274,7 +2274,7 @@
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="0"/>
-        <v>100028</v>
+        <v>100026</v>
       </c>
       <c r="C27" t="s">
         <v>22</v>
@@ -2296,7 +2296,7 @@
       </c>
       <c r="I27">
         <f t="shared" ca="1" si="1"/>
-        <v>250</v>
+        <v>52</v>
       </c>
       <c r="J27">
         <v>1</v>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="O27">
         <f t="shared" ca="1" si="2"/>
-        <v>4403</v>
+        <v>5732</v>
       </c>
       <c r="P27">
         <v>2</v>
@@ -2327,7 +2327,7 @@
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="0"/>
-        <v>100016</v>
+        <v>100025</v>
       </c>
       <c r="C28" t="s">
         <v>20</v>
@@ -2349,7 +2349,7 @@
       </c>
       <c r="I28">
         <f t="shared" ca="1" si="1"/>
-        <v>128</v>
+        <v>27</v>
       </c>
       <c r="J28">
         <v>1</v>
@@ -2368,7 +2368,7 @@
       </c>
       <c r="O28">
         <f t="shared" ca="1" si="2"/>
-        <v>2356</v>
+        <v>933</v>
       </c>
       <c r="P28">
         <v>1</v>
@@ -2380,7 +2380,7 @@
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="0"/>
-        <v>100002</v>
+        <v>100022</v>
       </c>
       <c r="C29" t="s">
         <v>20</v>
@@ -2402,7 +2402,7 @@
       </c>
       <c r="I29">
         <f t="shared" ca="1" si="1"/>
-        <v>226</v>
+        <v>129</v>
       </c>
       <c r="J29">
         <v>1</v>
@@ -2421,7 +2421,7 @@
       </c>
       <c r="O29">
         <f t="shared" ca="1" si="2"/>
-        <v>3274</v>
+        <v>2271</v>
       </c>
       <c r="P29">
         <v>1</v>
@@ -2433,7 +2433,7 @@
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="0"/>
-        <v>100011</v>
+        <v>100008</v>
       </c>
       <c r="C30" t="s">
         <v>17</v>
@@ -2481,7 +2481,7 @@
       </c>
       <c r="B31">
         <f t="shared" ca="1" si="0"/>
-        <v>100028</v>
+        <v>100006</v>
       </c>
       <c r="C31" t="s">
         <v>17</v>
@@ -2532,7 +2532,7 @@
       </c>
       <c r="B32">
         <f t="shared" ca="1" si="0"/>
-        <v>100006</v>
+        <v>100002</v>
       </c>
       <c r="C32" t="s">
         <v>17</v>
@@ -2628,7 +2628,7 @@
       </c>
       <c r="B34">
         <f t="shared" ca="1" si="0"/>
-        <v>100023</v>
+        <v>100005</v>
       </c>
       <c r="C34" t="s">
         <v>22</v>
@@ -2730,7 +2730,7 @@
       </c>
       <c r="B36">
         <f t="shared" ca="1" si="0"/>
-        <v>100016</v>
+        <v>100026</v>
       </c>
       <c r="C36" t="s">
         <v>20</v>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="B37">
         <f t="shared" ca="1" si="0"/>
-        <v>100012</v>
+        <v>100018</v>
       </c>
       <c r="C37" t="s">
         <v>17</v>
@@ -2803,7 +2803,7 @@
       </c>
       <c r="I37">
         <f ca="1">RANDBETWEEN(20,300)</f>
-        <v>164</v>
+        <v>119</v>
       </c>
       <c r="J37">
         <v>1</v>
@@ -2819,7 +2819,7 @@
       </c>
       <c r="O37">
         <f ca="1">RANDBETWEEN(200,6000)</f>
-        <v>747</v>
+        <v>899</v>
       </c>
       <c r="P37">
         <v>1</v>
@@ -2831,7 +2831,7 @@
       </c>
       <c r="B38">
         <f t="shared" ca="1" si="0"/>
-        <v>100006</v>
+        <v>100010</v>
       </c>
       <c r="C38" t="s">
         <v>17</v>
@@ -2853,7 +2853,7 @@
       </c>
       <c r="I38">
         <f t="shared" ref="I38:I51" ca="1" si="3">RANDBETWEEN(20,300)</f>
-        <v>158</v>
+        <v>87</v>
       </c>
       <c r="J38">
         <v>1</v>
@@ -2869,7 +2869,7 @@
       </c>
       <c r="O38">
         <f t="shared" ref="O38:O51" ca="1" si="4">RANDBETWEEN(200,6000)</f>
-        <v>5945</v>
+        <v>5852</v>
       </c>
       <c r="P38">
         <v>1</v>
@@ -2881,7 +2881,7 @@
       </c>
       <c r="B39">
         <f t="shared" ca="1" si="0"/>
-        <v>100011</v>
+        <v>100025</v>
       </c>
       <c r="C39" t="s">
         <v>17</v>
@@ -2903,7 +2903,7 @@
       </c>
       <c r="I39">
         <f t="shared" ca="1" si="3"/>
-        <v>30</v>
+        <v>195</v>
       </c>
       <c r="J39">
         <v>1</v>
@@ -2919,7 +2919,7 @@
       </c>
       <c r="O39">
         <f t="shared" ca="1" si="4"/>
-        <v>2954</v>
+        <v>3046</v>
       </c>
       <c r="P39">
         <v>2</v>
@@ -2934,7 +2934,7 @@
       </c>
       <c r="B40">
         <f t="shared" ca="1" si="0"/>
-        <v>100007</v>
+        <v>100021</v>
       </c>
       <c r="C40" t="s">
         <v>20</v>
@@ -2956,7 +2956,7 @@
       </c>
       <c r="I40">
         <f t="shared" ca="1" si="3"/>
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="J40">
         <v>1</v>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="O40">
         <f t="shared" ca="1" si="4"/>
-        <v>5121</v>
+        <v>5584</v>
       </c>
       <c r="P40">
         <v>1</v>
@@ -2987,7 +2987,7 @@
       </c>
       <c r="B41">
         <f t="shared" ca="1" si="0"/>
-        <v>100002</v>
+        <v>100021</v>
       </c>
       <c r="C41" t="s">
         <v>20</v>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="I41">
         <f t="shared" ca="1" si="3"/>
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="J41">
         <v>1</v>
@@ -3028,7 +3028,7 @@
       </c>
       <c r="O41">
         <f t="shared" ca="1" si="4"/>
-        <v>5786</v>
+        <v>4399</v>
       </c>
       <c r="P41">
         <v>1</v>
@@ -3040,7 +3040,7 @@
       </c>
       <c r="B42">
         <f t="shared" ca="1" si="0"/>
-        <v>100014</v>
+        <v>100017</v>
       </c>
       <c r="C42" t="s">
         <v>20</v>
@@ -3062,7 +3062,7 @@
       </c>
       <c r="I42">
         <f t="shared" ca="1" si="3"/>
-        <v>213</v>
+        <v>132</v>
       </c>
       <c r="J42">
         <v>1</v>
@@ -3081,7 +3081,7 @@
       </c>
       <c r="O42">
         <f t="shared" ca="1" si="4"/>
-        <v>4082</v>
+        <v>3550</v>
       </c>
       <c r="P42">
         <v>1</v>
@@ -3093,7 +3093,7 @@
       </c>
       <c r="B43">
         <f t="shared" ca="1" si="0"/>
-        <v>100028</v>
+        <v>100006</v>
       </c>
       <c r="C43" t="s">
         <v>20</v>
@@ -3115,7 +3115,7 @@
       </c>
       <c r="I43">
         <f t="shared" ca="1" si="3"/>
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J43">
         <v>1</v>
@@ -3134,7 +3134,7 @@
       </c>
       <c r="O43">
         <f t="shared" ca="1" si="4"/>
-        <v>507</v>
+        <v>1449</v>
       </c>
       <c r="P43">
         <v>1</v>
@@ -3146,7 +3146,7 @@
       </c>
       <c r="B44">
         <f t="shared" ca="1" si="0"/>
-        <v>100025</v>
+        <v>100018</v>
       </c>
       <c r="C44" t="s">
         <v>17</v>
@@ -3168,7 +3168,7 @@
       </c>
       <c r="I44">
         <f t="shared" ca="1" si="3"/>
-        <v>190</v>
+        <v>22</v>
       </c>
       <c r="J44">
         <v>1</v>
@@ -3184,7 +3184,7 @@
       </c>
       <c r="O44">
         <f t="shared" ca="1" si="4"/>
-        <v>2121</v>
+        <v>1494</v>
       </c>
       <c r="P44">
         <v>1</v>
@@ -3196,7 +3196,7 @@
       </c>
       <c r="B45">
         <f t="shared" ca="1" si="0"/>
-        <v>100014</v>
+        <v>100027</v>
       </c>
       <c r="C45" t="s">
         <v>17</v>
@@ -3218,7 +3218,7 @@
       </c>
       <c r="I45">
         <f t="shared" ca="1" si="3"/>
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="J45">
         <v>1</v>
@@ -3234,7 +3234,7 @@
       </c>
       <c r="O45">
         <f t="shared" ca="1" si="4"/>
-        <v>5642</v>
+        <v>1876</v>
       </c>
       <c r="P45">
         <v>2</v>
@@ -3271,7 +3271,7 @@
       </c>
       <c r="I46">
         <f t="shared" ca="1" si="3"/>
-        <v>294</v>
+        <v>36</v>
       </c>
       <c r="J46">
         <v>1</v>
@@ -3287,7 +3287,7 @@
       </c>
       <c r="O46">
         <f t="shared" ca="1" si="4"/>
-        <v>4998</v>
+        <v>5747</v>
       </c>
       <c r="P46">
         <v>1</v>
@@ -3299,7 +3299,7 @@
       </c>
       <c r="B47">
         <f t="shared" ca="1" si="0"/>
-        <v>100023</v>
+        <v>100026</v>
       </c>
       <c r="C47" t="s">
         <v>22</v>
@@ -3321,7 +3321,7 @@
       </c>
       <c r="I47">
         <f t="shared" ca="1" si="3"/>
-        <v>270</v>
+        <v>50</v>
       </c>
       <c r="J47">
         <v>1</v>
@@ -3337,7 +3337,7 @@
       </c>
       <c r="O47">
         <f t="shared" ca="1" si="4"/>
-        <v>5760</v>
+        <v>284</v>
       </c>
       <c r="P47">
         <v>1</v>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="B48">
         <f t="shared" ca="1" si="0"/>
-        <v>100018</v>
+        <v>100004</v>
       </c>
       <c r="C48" t="s">
         <v>22</v>
@@ -3371,7 +3371,7 @@
       </c>
       <c r="I48">
         <f t="shared" ca="1" si="3"/>
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="J48">
         <v>1</v>
@@ -3387,7 +3387,7 @@
       </c>
       <c r="O48">
         <f t="shared" ca="1" si="4"/>
-        <v>3124</v>
+        <v>5916</v>
       </c>
       <c r="P48">
         <v>2</v>
@@ -3402,7 +3402,7 @@
       </c>
       <c r="B49">
         <f t="shared" ca="1" si="0"/>
-        <v>100001</v>
+        <v>100006</v>
       </c>
       <c r="C49" t="s">
         <v>20</v>
@@ -3424,7 +3424,7 @@
       </c>
       <c r="I49">
         <f t="shared" ca="1" si="3"/>
-        <v>54</v>
+        <v>245</v>
       </c>
       <c r="J49">
         <v>1</v>
@@ -3443,7 +3443,7 @@
       </c>
       <c r="O49">
         <f t="shared" ca="1" si="4"/>
-        <v>2184</v>
+        <v>4207</v>
       </c>
       <c r="P49">
         <v>1</v>
@@ -3455,7 +3455,7 @@
       </c>
       <c r="B50">
         <f t="shared" ca="1" si="0"/>
-        <v>100004</v>
+        <v>100026</v>
       </c>
       <c r="C50" t="s">
         <v>20</v>
@@ -3477,7 +3477,7 @@
       </c>
       <c r="I50">
         <f t="shared" ca="1" si="3"/>
-        <v>135</v>
+        <v>54</v>
       </c>
       <c r="J50">
         <v>1</v>
@@ -3496,7 +3496,7 @@
       </c>
       <c r="O50">
         <f t="shared" ca="1" si="4"/>
-        <v>5624</v>
+        <v>5668</v>
       </c>
       <c r="P50">
         <v>1</v>
@@ -3508,7 +3508,7 @@
       </c>
       <c r="B51">
         <f t="shared" ca="1" si="0"/>
-        <v>100001</v>
+        <v>100015</v>
       </c>
       <c r="C51" t="s">
         <v>20</v>
@@ -3530,7 +3530,7 @@
       </c>
       <c r="I51">
         <f t="shared" ca="1" si="3"/>
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="J51">
         <v>1</v>
@@ -3549,7 +3549,7 @@
       </c>
       <c r="O51">
         <f t="shared" ca="1" si="4"/>
-        <v>4398</v>
+        <v>1546</v>
       </c>
       <c r="P51">
         <v>1</v>
@@ -3561,7 +3561,7 @@
       </c>
       <c r="B52">
         <f t="shared" ca="1" si="0"/>
-        <v>100017</v>
+        <v>100001</v>
       </c>
       <c r="C52" t="s">
         <v>17</v>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="B53">
         <f t="shared" ca="1" si="0"/>
-        <v>100015</v>
+        <v>100011</v>
       </c>
       <c r="C53" t="s">
         <v>17</v>
@@ -3657,7 +3657,7 @@
       </c>
       <c r="B54">
         <f t="shared" ca="1" si="0"/>
-        <v>100008</v>
+        <v>100030</v>
       </c>
       <c r="C54" t="s">
         <v>17</v>
@@ -3708,7 +3708,7 @@
       </c>
       <c r="B55">
         <f t="shared" ca="1" si="0"/>
-        <v>100002</v>
+        <v>100024</v>
       </c>
       <c r="C55" t="s">
         <v>20</v>
@@ -3759,7 +3759,7 @@
       </c>
       <c r="B56">
         <f t="shared" ca="1" si="0"/>
-        <v>100017</v>
+        <v>100025</v>
       </c>
       <c r="C56" t="s">
         <v>20</v>
@@ -3810,7 +3810,7 @@
       </c>
       <c r="B57">
         <f t="shared" ca="1" si="0"/>
-        <v>100019</v>
+        <v>100022</v>
       </c>
       <c r="C57" t="s">
         <v>20</v>
@@ -3861,7 +3861,7 @@
       </c>
       <c r="B58">
         <f t="shared" ca="1" si="0"/>
-        <v>100030</v>
+        <v>100010</v>
       </c>
       <c r="C58" t="s">
         <v>20</v>
@@ -3912,7 +3912,7 @@
       </c>
       <c r="B59">
         <f t="shared" ca="1" si="0"/>
-        <v>100004</v>
+        <v>100018</v>
       </c>
       <c r="C59" t="s">
         <v>17</v>
@@ -3960,7 +3960,7 @@
       </c>
       <c r="B60">
         <f t="shared" ca="1" si="0"/>
-        <v>100029</v>
+        <v>100013</v>
       </c>
       <c r="C60" t="s">
         <v>17</v>
@@ -4011,7 +4011,7 @@
       </c>
       <c r="B61">
         <f t="shared" ca="1" si="0"/>
-        <v>100028</v>
+        <v>100029</v>
       </c>
       <c r="C61" t="s">
         <v>17</v>
@@ -4059,7 +4059,7 @@
       </c>
       <c r="B62">
         <f t="shared" ca="1" si="0"/>
-        <v>100014</v>
+        <v>100021</v>
       </c>
       <c r="C62" t="s">
         <v>22</v>
@@ -4107,7 +4107,7 @@
       </c>
       <c r="B63">
         <f t="shared" ca="1" si="0"/>
-        <v>100019</v>
+        <v>100026</v>
       </c>
       <c r="C63" t="s">
         <v>22</v>
@@ -4158,7 +4158,7 @@
       </c>
       <c r="B64">
         <f t="shared" ca="1" si="0"/>
-        <v>100008</v>
+        <v>100013</v>
       </c>
       <c r="C64" t="s">
         <v>20</v>
@@ -4209,7 +4209,7 @@
       </c>
       <c r="B65">
         <f t="shared" ca="1" si="0"/>
-        <v>100014</v>
+        <v>100011</v>
       </c>
       <c r="C65" t="s">
         <v>20</v>
@@ -4260,7 +4260,7 @@
       </c>
       <c r="B66">
         <f t="shared" ca="1" si="0"/>
-        <v>100002</v>
+        <v>100017</v>
       </c>
       <c r="C66" t="s">
         <v>17</v>
@@ -4282,7 +4282,7 @@
       </c>
       <c r="I66">
         <f ca="1">RANDBETWEEN(20,300)</f>
-        <v>67</v>
+        <v>210</v>
       </c>
       <c r="J66">
         <v>1</v>
@@ -4298,7 +4298,7 @@
       </c>
       <c r="O66">
         <f ca="1">RANDBETWEEN(200,6000)</f>
-        <v>5038</v>
+        <v>1958</v>
       </c>
       <c r="P66">
         <v>1</v>
@@ -4310,7 +4310,7 @@
       </c>
       <c r="B67">
         <f t="shared" ref="B67:B101" ca="1" si="5">RANDBETWEEN(100001,100030)</f>
-        <v>100010</v>
+        <v>100003</v>
       </c>
       <c r="C67" t="s">
         <v>17</v>
@@ -4332,7 +4332,7 @@
       </c>
       <c r="I67">
         <f t="shared" ref="I67:I79" ca="1" si="6">RANDBETWEEN(20,300)</f>
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="J67">
         <v>1</v>
@@ -4348,7 +4348,7 @@
       </c>
       <c r="O67">
         <f t="shared" ref="O67:O79" ca="1" si="7">RANDBETWEEN(200,6000)</f>
-        <v>5667</v>
+        <v>2351</v>
       </c>
       <c r="P67">
         <v>1</v>
@@ -4360,7 +4360,7 @@
       </c>
       <c r="B68">
         <f t="shared" ca="1" si="5"/>
-        <v>100018</v>
+        <v>100027</v>
       </c>
       <c r="C68" t="s">
         <v>17</v>
@@ -4382,7 +4382,7 @@
       </c>
       <c r="I68">
         <f t="shared" ca="1" si="6"/>
-        <v>199</v>
+        <v>21</v>
       </c>
       <c r="J68">
         <v>1</v>
@@ -4398,7 +4398,7 @@
       </c>
       <c r="O68">
         <f t="shared" ca="1" si="7"/>
-        <v>4248</v>
+        <v>993</v>
       </c>
       <c r="P68">
         <v>2</v>
@@ -4413,7 +4413,7 @@
       </c>
       <c r="B69">
         <f t="shared" ca="1" si="5"/>
-        <v>100005</v>
+        <v>100015</v>
       </c>
       <c r="C69" t="s">
         <v>20</v>
@@ -4435,7 +4435,7 @@
       </c>
       <c r="I69">
         <f t="shared" ca="1" si="6"/>
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="J69">
         <v>1</v>
@@ -4454,7 +4454,7 @@
       </c>
       <c r="O69">
         <f t="shared" ca="1" si="7"/>
-        <v>3929</v>
+        <v>4217</v>
       </c>
       <c r="P69">
         <v>1</v>
@@ -4466,7 +4466,7 @@
       </c>
       <c r="B70">
         <f t="shared" ca="1" si="5"/>
-        <v>100005</v>
+        <v>100021</v>
       </c>
       <c r="C70" t="s">
         <v>20</v>
@@ -4488,7 +4488,7 @@
       </c>
       <c r="I70">
         <f t="shared" ca="1" si="6"/>
-        <v>116</v>
+        <v>289</v>
       </c>
       <c r="J70">
         <v>1</v>
@@ -4507,7 +4507,7 @@
       </c>
       <c r="O70">
         <f t="shared" ca="1" si="7"/>
-        <v>2478</v>
+        <v>2538</v>
       </c>
       <c r="P70">
         <v>1</v>
@@ -4519,7 +4519,7 @@
       </c>
       <c r="B71">
         <f t="shared" ca="1" si="5"/>
-        <v>100002</v>
+        <v>100008</v>
       </c>
       <c r="C71" t="s">
         <v>20</v>
@@ -4541,7 +4541,7 @@
       </c>
       <c r="I71">
         <f t="shared" ca="1" si="6"/>
-        <v>163</v>
+        <v>192</v>
       </c>
       <c r="J71">
         <v>1</v>
@@ -4560,7 +4560,7 @@
       </c>
       <c r="O71">
         <f t="shared" ca="1" si="7"/>
-        <v>5301</v>
+        <v>1763</v>
       </c>
       <c r="P71">
         <v>1</v>
@@ -4572,7 +4572,7 @@
       </c>
       <c r="B72">
         <f t="shared" ca="1" si="5"/>
-        <v>100016</v>
+        <v>100006</v>
       </c>
       <c r="C72" t="s">
         <v>20</v>
@@ -4594,7 +4594,7 @@
       </c>
       <c r="I72">
         <f t="shared" ca="1" si="6"/>
-        <v>229</v>
+        <v>76</v>
       </c>
       <c r="J72">
         <v>1</v>
@@ -4613,7 +4613,7 @@
       </c>
       <c r="O72">
         <f t="shared" ca="1" si="7"/>
-        <v>1012</v>
+        <v>5423</v>
       </c>
       <c r="P72">
         <v>1</v>
@@ -4625,7 +4625,7 @@
       </c>
       <c r="B73">
         <f t="shared" ca="1" si="5"/>
-        <v>100014</v>
+        <v>100023</v>
       </c>
       <c r="C73" t="s">
         <v>17</v>
@@ -4647,7 +4647,7 @@
       </c>
       <c r="I73">
         <f t="shared" ca="1" si="6"/>
-        <v>232</v>
+        <v>43</v>
       </c>
       <c r="J73">
         <v>1</v>
@@ -4663,7 +4663,7 @@
       </c>
       <c r="O73">
         <f t="shared" ca="1" si="7"/>
-        <v>3998</v>
+        <v>2786</v>
       </c>
       <c r="P73">
         <v>1</v>
@@ -4675,7 +4675,7 @@
       </c>
       <c r="B74">
         <f t="shared" ca="1" si="5"/>
-        <v>100018</v>
+        <v>100010</v>
       </c>
       <c r="C74" t="s">
         <v>17</v>
@@ -4697,7 +4697,7 @@
       </c>
       <c r="I74">
         <f t="shared" ca="1" si="6"/>
-        <v>190</v>
+        <v>288</v>
       </c>
       <c r="J74">
         <v>1</v>
@@ -4713,7 +4713,7 @@
       </c>
       <c r="O74">
         <f t="shared" ca="1" si="7"/>
-        <v>1419</v>
+        <v>2528</v>
       </c>
       <c r="P74">
         <v>2</v>
@@ -4728,7 +4728,7 @@
       </c>
       <c r="B75">
         <f t="shared" ca="1" si="5"/>
-        <v>100016</v>
+        <v>100006</v>
       </c>
       <c r="C75" t="s">
         <v>17</v>
@@ -4750,7 +4750,7 @@
       </c>
       <c r="I75">
         <f t="shared" ca="1" si="6"/>
-        <v>251</v>
+        <v>35</v>
       </c>
       <c r="J75">
         <v>1</v>
@@ -4766,7 +4766,7 @@
       </c>
       <c r="O75">
         <f t="shared" ca="1" si="7"/>
-        <v>1717</v>
+        <v>1910</v>
       </c>
       <c r="P75">
         <v>1</v>
@@ -4778,7 +4778,7 @@
       </c>
       <c r="B76">
         <f t="shared" ca="1" si="5"/>
-        <v>100012</v>
+        <v>100009</v>
       </c>
       <c r="C76" t="s">
         <v>22</v>
@@ -4800,7 +4800,7 @@
       </c>
       <c r="I76">
         <f t="shared" ca="1" si="6"/>
-        <v>126</v>
+        <v>100</v>
       </c>
       <c r="J76">
         <v>1</v>
@@ -4816,7 +4816,7 @@
       </c>
       <c r="O76">
         <f t="shared" ca="1" si="7"/>
-        <v>2191</v>
+        <v>5892</v>
       </c>
       <c r="P76">
         <v>1</v>
@@ -4828,7 +4828,7 @@
       </c>
       <c r="B77">
         <f t="shared" ca="1" si="5"/>
-        <v>100010</v>
+        <v>100021</v>
       </c>
       <c r="C77" t="s">
         <v>22</v>
@@ -4850,7 +4850,7 @@
       </c>
       <c r="I77">
         <f t="shared" ca="1" si="6"/>
-        <v>165</v>
+        <v>253</v>
       </c>
       <c r="J77">
         <v>1</v>
@@ -4866,7 +4866,7 @@
       </c>
       <c r="O77">
         <f t="shared" ca="1" si="7"/>
-        <v>2685</v>
+        <v>1848</v>
       </c>
       <c r="P77">
         <v>2</v>
@@ -4903,7 +4903,7 @@
       </c>
       <c r="I78">
         <f t="shared" ca="1" si="6"/>
-        <v>248</v>
+        <v>194</v>
       </c>
       <c r="J78">
         <v>1</v>
@@ -4922,7 +4922,7 @@
       </c>
       <c r="O78">
         <f t="shared" ca="1" si="7"/>
-        <v>1338</v>
+        <v>2424</v>
       </c>
       <c r="P78">
         <v>1</v>
@@ -4934,7 +4934,7 @@
       </c>
       <c r="B79">
         <f t="shared" ca="1" si="5"/>
-        <v>100016</v>
+        <v>100013</v>
       </c>
       <c r="C79" t="s">
         <v>20</v>
@@ -4956,7 +4956,7 @@
       </c>
       <c r="I79">
         <f t="shared" ca="1" si="6"/>
-        <v>65</v>
+        <v>255</v>
       </c>
       <c r="J79">
         <v>1</v>
@@ -4975,7 +4975,7 @@
       </c>
       <c r="O79">
         <f t="shared" ca="1" si="7"/>
-        <v>4518</v>
+        <v>3322</v>
       </c>
       <c r="P79">
         <v>1</v>
@@ -4987,7 +4987,7 @@
       </c>
       <c r="B80">
         <f t="shared" ca="1" si="5"/>
-        <v>100023</v>
+        <v>100021</v>
       </c>
       <c r="C80" t="s">
         <v>17</v>
@@ -5035,7 +5035,7 @@
       </c>
       <c r="B81">
         <f t="shared" ca="1" si="5"/>
-        <v>100012</v>
+        <v>100024</v>
       </c>
       <c r="C81" t="s">
         <v>17</v>
@@ -5086,7 +5086,7 @@
       </c>
       <c r="B82">
         <f t="shared" ca="1" si="5"/>
-        <v>100003</v>
+        <v>100006</v>
       </c>
       <c r="C82" t="s">
         <v>17</v>
@@ -5134,7 +5134,7 @@
       </c>
       <c r="B83">
         <f t="shared" ca="1" si="5"/>
-        <v>100004</v>
+        <v>100007</v>
       </c>
       <c r="C83" t="s">
         <v>22</v>
@@ -5182,7 +5182,7 @@
       </c>
       <c r="B84">
         <f t="shared" ca="1" si="5"/>
-        <v>100009</v>
+        <v>100025</v>
       </c>
       <c r="C84" t="s">
         <v>22</v>
@@ -5233,7 +5233,7 @@
       </c>
       <c r="B85">
         <f t="shared" ca="1" si="5"/>
-        <v>100009</v>
+        <v>100018</v>
       </c>
       <c r="C85" t="s">
         <v>20</v>
@@ -5284,7 +5284,7 @@
       </c>
       <c r="B86">
         <f t="shared" ca="1" si="5"/>
-        <v>100009</v>
+        <v>100029</v>
       </c>
       <c r="C86" t="s">
         <v>20</v>
@@ -5335,7 +5335,7 @@
       </c>
       <c r="B87">
         <f t="shared" ca="1" si="5"/>
-        <v>100003</v>
+        <v>100022</v>
       </c>
       <c r="C87" t="s">
         <v>17</v>
@@ -5357,7 +5357,7 @@
       </c>
       <c r="I87">
         <f ca="1">RANDBETWEEN(20,300)</f>
-        <v>278</v>
+        <v>44</v>
       </c>
       <c r="J87">
         <v>1</v>
@@ -5373,7 +5373,7 @@
       </c>
       <c r="O87">
         <f ca="1">RANDBETWEEN(200,6000)</f>
-        <v>4259</v>
+        <v>1663</v>
       </c>
       <c r="P87">
         <v>1</v>
@@ -5407,7 +5407,7 @@
       </c>
       <c r="I88">
         <f t="shared" ref="I88:I101" ca="1" si="8">RANDBETWEEN(20,300)</f>
-        <v>135</v>
+        <v>299</v>
       </c>
       <c r="J88">
         <v>1</v>
@@ -5423,7 +5423,7 @@
       </c>
       <c r="O88">
         <f t="shared" ref="O88:O101" ca="1" si="9">RANDBETWEEN(200,6000)</f>
-        <v>2046</v>
+        <v>4049</v>
       </c>
       <c r="P88">
         <v>1</v>
@@ -5435,7 +5435,7 @@
       </c>
       <c r="B89">
         <f t="shared" ca="1" si="5"/>
-        <v>100005</v>
+        <v>100013</v>
       </c>
       <c r="C89" t="s">
         <v>17</v>
@@ -5457,7 +5457,7 @@
       </c>
       <c r="I89">
         <f t="shared" ca="1" si="8"/>
-        <v>272</v>
+        <v>179</v>
       </c>
       <c r="J89">
         <v>1</v>
@@ -5473,7 +5473,7 @@
       </c>
       <c r="O89">
         <f t="shared" ca="1" si="9"/>
-        <v>3343</v>
+        <v>777</v>
       </c>
       <c r="P89">
         <v>2</v>
@@ -5488,7 +5488,7 @@
       </c>
       <c r="B90">
         <f t="shared" ca="1" si="5"/>
-        <v>100015</v>
+        <v>100028</v>
       </c>
       <c r="C90" t="s">
         <v>20</v>
@@ -5510,7 +5510,7 @@
       </c>
       <c r="I90">
         <f t="shared" ca="1" si="8"/>
-        <v>245</v>
+        <v>77</v>
       </c>
       <c r="J90">
         <v>1</v>
@@ -5529,7 +5529,7 @@
       </c>
       <c r="O90">
         <f t="shared" ca="1" si="9"/>
-        <v>5596</v>
+        <v>4938</v>
       </c>
       <c r="P90">
         <v>1</v>
@@ -5541,7 +5541,7 @@
       </c>
       <c r="B91">
         <f t="shared" ca="1" si="5"/>
-        <v>100013</v>
+        <v>100023</v>
       </c>
       <c r="C91" t="s">
         <v>20</v>
@@ -5563,7 +5563,7 @@
       </c>
       <c r="I91">
         <f t="shared" ca="1" si="8"/>
-        <v>130</v>
+        <v>249</v>
       </c>
       <c r="J91">
         <v>1</v>
@@ -5582,7 +5582,7 @@
       </c>
       <c r="O91">
         <f t="shared" ca="1" si="9"/>
-        <v>5454</v>
+        <v>4476</v>
       </c>
       <c r="P91">
         <v>1</v>
@@ -5594,7 +5594,7 @@
       </c>
       <c r="B92">
         <f t="shared" ca="1" si="5"/>
-        <v>100010</v>
+        <v>100020</v>
       </c>
       <c r="C92" t="s">
         <v>20</v>
@@ -5616,7 +5616,7 @@
       </c>
       <c r="I92">
         <f t="shared" ca="1" si="8"/>
-        <v>156</v>
+        <v>282</v>
       </c>
       <c r="J92">
         <v>1</v>
@@ -5635,7 +5635,7 @@
       </c>
       <c r="O92">
         <f t="shared" ca="1" si="9"/>
-        <v>4613</v>
+        <v>2121</v>
       </c>
       <c r="P92">
         <v>1</v>
@@ -5647,7 +5647,7 @@
       </c>
       <c r="B93">
         <f t="shared" ca="1" si="5"/>
-        <v>100009</v>
+        <v>100001</v>
       </c>
       <c r="C93" t="s">
         <v>20</v>
@@ -5669,7 +5669,7 @@
       </c>
       <c r="I93">
         <f t="shared" ca="1" si="8"/>
-        <v>60</v>
+        <v>114</v>
       </c>
       <c r="J93">
         <v>1</v>
@@ -5688,7 +5688,7 @@
       </c>
       <c r="O93">
         <f t="shared" ca="1" si="9"/>
-        <v>3662</v>
+        <v>2104</v>
       </c>
       <c r="P93">
         <v>1</v>
@@ -5700,7 +5700,7 @@
       </c>
       <c r="B94">
         <f t="shared" ca="1" si="5"/>
-        <v>100030</v>
+        <v>100009</v>
       </c>
       <c r="C94" t="s">
         <v>17</v>
@@ -5722,7 +5722,7 @@
       </c>
       <c r="I94">
         <f t="shared" ca="1" si="8"/>
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="J94">
         <v>1</v>
@@ -5738,7 +5738,7 @@
       </c>
       <c r="O94">
         <f t="shared" ca="1" si="9"/>
-        <v>1712</v>
+        <v>4795</v>
       </c>
       <c r="P94">
         <v>1</v>
@@ -5750,7 +5750,7 @@
       </c>
       <c r="B95">
         <f t="shared" ca="1" si="5"/>
-        <v>100022</v>
+        <v>100003</v>
       </c>
       <c r="C95" t="s">
         <v>17</v>
@@ -5772,7 +5772,7 @@
       </c>
       <c r="I95">
         <f t="shared" ca="1" si="8"/>
-        <v>27</v>
+        <v>135</v>
       </c>
       <c r="J95">
         <v>1</v>
@@ -5788,7 +5788,7 @@
       </c>
       <c r="O95">
         <f t="shared" ca="1" si="9"/>
-        <v>1592</v>
+        <v>4454</v>
       </c>
       <c r="P95">
         <v>2</v>
@@ -5803,7 +5803,7 @@
       </c>
       <c r="B96">
         <f t="shared" ca="1" si="5"/>
-        <v>100007</v>
+        <v>100029</v>
       </c>
       <c r="C96" t="s">
         <v>17</v>
@@ -5825,7 +5825,7 @@
       </c>
       <c r="I96">
         <f t="shared" ca="1" si="8"/>
-        <v>212</v>
+        <v>291</v>
       </c>
       <c r="J96">
         <v>1</v>
@@ -5841,7 +5841,7 @@
       </c>
       <c r="O96">
         <f t="shared" ca="1" si="9"/>
-        <v>1086</v>
+        <v>2915</v>
       </c>
       <c r="P96">
         <v>1</v>
@@ -5853,7 +5853,7 @@
       </c>
       <c r="B97">
         <f t="shared" ca="1" si="5"/>
-        <v>100003</v>
+        <v>100004</v>
       </c>
       <c r="C97" t="s">
         <v>22</v>
@@ -5875,7 +5875,7 @@
       </c>
       <c r="I97">
         <f t="shared" ca="1" si="8"/>
-        <v>82</v>
+        <v>249</v>
       </c>
       <c r="J97">
         <v>1</v>
@@ -5891,7 +5891,7 @@
       </c>
       <c r="O97">
         <f t="shared" ca="1" si="9"/>
-        <v>3727</v>
+        <v>2436</v>
       </c>
       <c r="P97">
         <v>1</v>
@@ -5903,7 +5903,7 @@
       </c>
       <c r="B98">
         <f t="shared" ca="1" si="5"/>
-        <v>100008</v>
+        <v>100023</v>
       </c>
       <c r="C98" t="s">
         <v>22</v>
@@ -5925,7 +5925,7 @@
       </c>
       <c r="I98">
         <f t="shared" ca="1" si="8"/>
-        <v>183</v>
+        <v>65</v>
       </c>
       <c r="J98">
         <v>1</v>
@@ -5941,7 +5941,7 @@
       </c>
       <c r="O98">
         <f t="shared" ca="1" si="9"/>
-        <v>3537</v>
+        <v>5958</v>
       </c>
       <c r="P98">
         <v>2</v>
@@ -5956,7 +5956,7 @@
       </c>
       <c r="B99">
         <f t="shared" ca="1" si="5"/>
-        <v>100005</v>
+        <v>100027</v>
       </c>
       <c r="C99" t="s">
         <v>20</v>
@@ -5978,7 +5978,7 @@
       </c>
       <c r="I99">
         <f t="shared" ca="1" si="8"/>
-        <v>137</v>
+        <v>190</v>
       </c>
       <c r="J99">
         <v>1</v>
@@ -5997,7 +5997,7 @@
       </c>
       <c r="O99">
         <f t="shared" ca="1" si="9"/>
-        <v>2591</v>
+        <v>5298</v>
       </c>
       <c r="P99">
         <v>1</v>
@@ -6031,7 +6031,7 @@
       </c>
       <c r="I100">
         <f t="shared" ca="1" si="8"/>
-        <v>143</v>
+        <v>236</v>
       </c>
       <c r="J100">
         <v>1</v>
@@ -6050,7 +6050,7 @@
       </c>
       <c r="O100">
         <f t="shared" ca="1" si="9"/>
-        <v>2062</v>
+        <v>2847</v>
       </c>
       <c r="P100">
         <v>1</v>
@@ -6062,7 +6062,7 @@
       </c>
       <c r="B101">
         <f t="shared" ca="1" si="5"/>
-        <v>100012</v>
+        <v>100010</v>
       </c>
       <c r="C101" t="s">
         <v>20</v>
@@ -6084,7 +6084,7 @@
       </c>
       <c r="I101">
         <f t="shared" ca="1" si="8"/>
-        <v>35</v>
+        <v>234</v>
       </c>
       <c r="J101">
         <v>1</v>
@@ -6103,7 +6103,7 @@
       </c>
       <c r="O101">
         <f t="shared" ca="1" si="9"/>
-        <v>5822</v>
+        <v>3862</v>
       </c>
       <c r="P101">
         <v>1</v>

</xml_diff>